<commit_message>
Finish the 3.0 version
</commit_message>
<xml_diff>
--- a/CCGroupSort/test.xlsx
+++ b/CCGroupSort/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,13 +150,21 @@
   </si>
   <si>
     <t>日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G学员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学员</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -723,6 +731,9 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
       <c r="L8" t="s">
         <v>24</v>
       </c>
@@ -740,10 +751,88 @@
       <c r="D9">
         <v>233</v>
       </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>233</v>
+      </c>
+      <c r="C10">
+        <v>233</v>
+      </c>
+      <c r="D10">
+        <v>233</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>233</v>
+      </c>
+      <c r="C11">
+        <v>233</v>
+      </c>
+      <c r="D11">
+        <v>233</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>233</v>
+      </c>
+      <c r="C12">
+        <v>233</v>
+      </c>
+      <c r="D12">
+        <v>233</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>